<commit_message>
#439: migrate styles and classes, fixes from testing, add actions for accordion/tabs
</commit_message>
<xml_diff>
--- a/examples/storage/test.xlsx
+++ b/examples/storage/test.xlsx
@@ -23,7 +23,7 @@
     <t>Actions</t>
   </si>
   <si>
-    <t>AarSvc_ca476</t>
+    <t>AarSvc_d97b7</t>
   </si>
   <si>
     <t>Stopped</t>
@@ -83,7 +83,7 @@
     <t>AxInstSV</t>
   </si>
   <si>
-    <t>BcastDVRUserService_ca476</t>
+    <t>BcastDVRUserService_d97b7</t>
   </si>
   <si>
     <t>BDESVC</t>
@@ -153,9 +153,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.4542675018311" customWidth="1"/>
+    <col min="1" max="1" width="26.775510787963867" customWidth="1"/>
     <col min="2" max="2" width="9.140625" customWidth="1"/>
-    <col min="3" max="3" width="10.158139705658" customWidth="1"/>
+    <col min="3" max="3" width="10.158139705657959" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -284,7 +284,7 @@
         <v>16</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>5</v>
@@ -372,7 +372,7 @@
         <v>24</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C20" s="0" t="s">
         <v>5</v>

</xml_diff>